<commit_message>
Add static folder and js
</commit_message>
<xml_diff>
--- a/user_files/hilarytn/line_3.xlsx
+++ b/user_files/hilarytn/line_3.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,7 +507,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H2" s="3" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H3" s="3" t="n">
@@ -575,7 +575,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H4" s="3" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H5" s="3" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H6" s="3" t="n">
@@ -677,7 +677,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H7" s="3" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H8" s="3" t="n">
@@ -745,10 +745,554 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9d7fe935-9ba4-4289-a505-a9d49b45ad9f</t>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
         </is>
       </c>
       <c r="H9" s="3" t="n">
+        <v>0.0002314814814814815</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SEC Cl</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45271.36145825232</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45271.36158556713</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0.0001273148148148148</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PRI pH</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45271.68537890046</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45271.68549464121</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45271.68549475694</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45271.68769383102</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>0.002199074074074074</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45271.6876965625</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45271.68898128472</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>0.001284722222222222</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH&amp;rem</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45271.68897129629</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45271.68908703703</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45271.6890871875</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45271.68920292824</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45271.89825825232</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>45271.8996471412</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>0.001388888888888889</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PRI Cl&amp;pH</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45272.09804105324</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>45272.09827253472</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>0.0002314814814814815</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SEC Cl</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45271.36145825232</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>45271.36158556713</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>0.0001273148148148148</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>PRI pH</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45271.68537890046</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>45271.68549464121</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45271.68549475694</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>45271.68769383102</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>0.002199074074074074</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45271.6876965625</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>45271.68898128472</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>0.001284722222222222</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH&amp;rem</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>45271.68897129629</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>45271.68908703703</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>45271.6890871875</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>45271.68920292824</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>45271.89825825232</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>45271.8996471412</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>0.001388888888888889</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>PRI Cl&amp;pH</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>45272.09804105324</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>45272.09827253472</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="n">
         <v>0.0002314814814814815</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create html files for version 2"
</commit_message>
<xml_diff>
--- a/user_files/hilarytn/line_3.xlsx
+++ b/user_files/hilarytn/line_3.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,7 +507,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H2" s="3" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H3" s="3" t="n">
@@ -575,7 +575,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H4" s="3" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H5" s="3" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H6" s="3" t="n">
@@ -677,7 +677,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H7" s="3" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H8" s="3" t="n">
@@ -745,7 +745,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H9" s="3" t="n">
@@ -779,7 +779,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H10" s="3" t="n">
@@ -813,7 +813,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H11" s="3" t="n">
@@ -847,7 +847,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H12" s="3" t="n">
@@ -881,7 +881,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H13" s="3" t="n">
@@ -915,7 +915,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H14" s="3" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H15" s="3" t="n">
@@ -983,7 +983,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H16" s="3" t="n">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H17" s="3" t="n">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H18" s="3" t="n">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H19" s="3" t="n">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H20" s="3" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H21" s="3" t="n">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H22" s="3" t="n">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H23" s="3" t="n">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H24" s="3" t="n">
@@ -1289,10 +1289,282 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>ddb71f0e-ca75-4b40-9ae2-33afa81c43ba</t>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
         </is>
       </c>
       <c r="H25" s="3" t="n">
+        <v>0.0002314814814814815</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SEC Cl</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45271.36145825232</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>45271.36158556713</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>0.0001273148148148148</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>PRI pH</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>45271.68537890046</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>45271.68549464121</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>45271.68549475694</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>45271.68769383102</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>0.002199074074074074</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>45271.6876965625</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>45271.68898128472</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>0.001284722222222222</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH&amp;rem</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45271.68897129629</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>45271.68908703703</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45271.6890871875</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>45271.68920292824</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>0.0001157407407407407</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>45271.89825825232</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>45271.8996471412</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>0.001388888888888889</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>PRI Cl&amp;pH</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>45272.09804105324</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>45272.09827253472</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>d85554b9-776c-49d1-bdf2-3016191cd60b</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="n">
         <v>0.0002314814814814815</v>
       </c>
     </row>

</xml_diff>